<commit_message>
refine club name matching and adjust participation points calculation with floor function
</commit_message>
<xml_diff>
--- a/data/season/current_season/Season_History.xlsx
+++ b/data/season/current_season/Season_History.xlsx
@@ -5604,7 +5604,7 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>South West Sydney Triathlon Club</t>
+          <t>Sydney South West Triathlon Club</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
@@ -5869,7 +5869,7 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>Balance Tri Club</t>
+          <t>Balance Triathlon Club</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
@@ -5922,7 +5922,7 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>Balance Tri Club</t>
+          <t>Balance Triathlon Club</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
@@ -5975,7 +5975,7 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>Balance Tri Club</t>
+          <t>Balance Triathlon Club</t>
         </is>
       </c>
       <c r="G105" t="inlineStr">
@@ -6028,7 +6028,7 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>Balance Tri Club</t>
+          <t>Balance Triathlon Club</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
@@ -6081,7 +6081,7 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>Balance Tri Club</t>
+          <t>Balance Triathlon Club</t>
         </is>
       </c>
       <c r="G107" t="inlineStr">
@@ -6134,7 +6134,7 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>Balance Tri Club</t>
+          <t>Balance Triathlon Club</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
@@ -6187,7 +6187,7 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>Balance Tri Club</t>
+          <t>Balance Triathlon Club</t>
         </is>
       </c>
       <c r="G109" t="inlineStr">
@@ -6240,7 +6240,7 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>Balance Tri Club</t>
+          <t>Balance Triathlon Club</t>
         </is>
       </c>
       <c r="G110" t="inlineStr">
@@ -6293,7 +6293,7 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>Balance Tri Club</t>
+          <t>Balance Triathlon Club</t>
         </is>
       </c>
       <c r="G111" t="inlineStr">
@@ -6346,7 +6346,7 @@
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>Balance Tri Club</t>
+          <t>Balance Triathlon Club</t>
         </is>
       </c>
       <c r="G112" t="inlineStr">
@@ -9314,7 +9314,7 @@
       </c>
       <c r="F168" t="inlineStr">
         <is>
-          <t>Balance Tri Club</t>
+          <t>Balance Triathlon Club</t>
         </is>
       </c>
       <c r="G168" t="inlineStr">
@@ -9367,7 +9367,7 @@
       </c>
       <c r="F169" t="inlineStr">
         <is>
-          <t>Balance Tri Club</t>
+          <t>Balance Triathlon Club</t>
         </is>
       </c>
       <c r="G169" t="inlineStr">
@@ -9420,7 +9420,7 @@
       </c>
       <c r="F170" t="inlineStr">
         <is>
-          <t>Balance Tri Club</t>
+          <t>Balance Triathlon Club</t>
         </is>
       </c>
       <c r="G170" t="inlineStr">
@@ -9473,7 +9473,7 @@
       </c>
       <c r="F171" t="inlineStr">
         <is>
-          <t>Balance Tri Club</t>
+          <t>Balance Triathlon Club</t>
         </is>
       </c>
       <c r="G171" t="inlineStr">

</xml_diff>